<commit_message>
Commit xsReduction - modified note about standard reduction number
</commit_message>
<xml_diff>
--- a/xsReduction.xlsx
+++ b/xsReduction.xlsx
@@ -31,7 +31,7 @@
             <family val="2"/>
           </rPr>
           <t>35 is standard for KCI XS report format
-Note that the first two and last two points are always kept</t>
+Note that the first two and last two points are kept no matter what</t>
         </r>
       </text>
     </comment>
@@ -6092,11 +6092,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="582518880"/>
-        <c:axId val="582518488"/>
+        <c:axId val="392259760"/>
+        <c:axId val="392251920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="582518880"/>
+        <c:axId val="392259760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6142,7 +6142,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6209,12 +6208,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="582518488"/>
+        <c:crossAx val="392251920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="582518488"/>
+        <c:axId val="392251920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6334,7 +6333,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="582518880"/>
+        <c:crossAx val="392259760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7305,7 +7304,7 @@
   <dimension ref="A1:V501"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>